<commit_message>
toy around with raw file stats
</commit_message>
<xml_diff>
--- a/tables_and_figures/Tables.xlsx
+++ b/tables_and_figures/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/tables_and_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{898FD414-F478-4643-A0E9-88FCC4A91679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE8226BA-DD4C-6342-8C54-366C1DF51E26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
   </bookViews>
@@ -534,9 +534,6 @@
     <t>Number of Bases</t>
   </si>
   <si>
-    <t>File Size</t>
-  </si>
-  <si>
     <t>Mean Read Length</t>
   </si>
   <si>
@@ -544,6 +541,9 @@
   </si>
   <si>
     <t>10X Illumina</t>
+  </si>
+  <si>
+    <t>File Size (fasta)</t>
   </si>
 </sst>
 </file>
@@ -3105,7 +3105,7 @@
   <dimension ref="B2:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3147,7 +3147,7 @@
         <v>46</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F3" s="26" t="s">
         <v>146</v>
@@ -3159,10 +3159,10 @@
         <v>144</v>
       </c>
       <c r="I3" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="J3" s="26" t="s">
         <v>148</v>
-      </c>
-      <c r="J3" s="26" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.2">
@@ -3307,7 +3307,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D9" s="14" t="s">
         <v>56</v>
@@ -3320,15 +3320,19 @@
       <c r="H9" s="15">
         <v>627984118</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="I9" s="14">
+        <v>151</v>
+      </c>
+      <c r="J9" s="14">
+        <v>33</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>57</v>
@@ -3341,15 +3345,19 @@
       <c r="H10" s="15">
         <v>627984118</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="I10" s="14">
+        <v>151</v>
+      </c>
+      <c r="J10" s="14">
+        <v>32</v>
+      </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>56</v>
@@ -3357,18 +3365,26 @@
       <c r="E11" s="15">
         <v>161450851775</v>
       </c>
-      <c r="F11" s="14"/>
+      <c r="F11" s="15">
+        <v>65806680934</v>
+      </c>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="15">
+        <v>435805834</v>
+      </c>
+      <c r="I11" s="14">
+        <v>151</v>
+      </c>
+      <c r="J11" s="14">
+        <v>34</v>
+      </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>57</v>
@@ -3376,11 +3392,19 @@
       <c r="E12" s="15">
         <v>161450851775</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="15">
+        <v>65806680934</v>
+      </c>
       <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="H12" s="15">
+        <v>435805834</v>
+      </c>
+      <c r="I12" s="14">
+        <v>151</v>
+      </c>
+      <c r="J12" s="14">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
up thru the beginning of cyto results
</commit_message>
<xml_diff>
--- a/tables_and_figures/Tables.xlsx
+++ b/tables_and_figures/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/tables_and_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81D3D8B7-C796-9D4D-BB35-39B0ABF2489C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFFB4AB-9E72-954F-A6B4-FF8E693732BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="5" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="6" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="TableTK_RawSeqStats" sheetId="5" r:id="rId4"/>
     <sheet name="TableTK_Seq_Metrics" sheetId="3" r:id="rId5"/>
     <sheet name="TableTK_AssemblyMetrics" sheetId="6" r:id="rId6"/>
+    <sheet name="TableTK_Cytogenetics" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="175">
   <si>
     <t>Total sequence length</t>
   </si>
@@ -562,9 +563,6 @@
     <t>Female</t>
   </si>
   <si>
-    <t>ipa</t>
-  </si>
-  <si>
     <t>L50</t>
   </si>
   <si>
@@ -586,22 +584,10 @@
     <t>fragmented</t>
   </si>
   <si>
-    <t>scaff10x</t>
-  </si>
-  <si>
-    <t>SALSA2</t>
-  </si>
-  <si>
-    <t>chromonomer</t>
-  </si>
-  <si>
     <t>Continuity Metrics</t>
   </si>
   <si>
     <t>total length</t>
-  </si>
-  <si>
-    <t>raw</t>
   </si>
   <si>
     <r>
@@ -618,12 +604,111 @@
       <t>Table of assembly steps with corresponding metrics. A0 = Metrics for unassembled, filtered PacBio HiFi reads; A1 = metrics after ipa assembly step; A2 = metrics afer scaffolding A1 assembly using linked-reads; A3 = metrics after scaffolding A2 assembly using hi-c data; A4 = metrics of final assembly resulting from anchoring chromosomes with a linkage map.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t># Cells</t>
+  </si>
+  <si>
+    <t>2n Count</t>
+  </si>
+  <si>
+    <t>Total # of Cells</t>
+  </si>
+  <si>
+    <r>
+      <t>Table TK.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> Chromosome counts for delta smelt indicating 2n = 56.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -744,6 +829,19 @@
       <name val="Calibri Light"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -771,7 +869,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -1087,32 +1185,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1154,12 +1230,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1175,6 +1295,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1273,46 +1396,31 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1321,9 +1429,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1360,7 +1465,7 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1371,6 +1476,36 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2106,368 +2241,368 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="32"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
-      <c r="R2" s="33"/>
-      <c r="S2" s="34"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="35"/>
     </row>
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B3" s="35"/>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="36"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="30"/>
+      <c r="O3" s="30"/>
+      <c r="P3" s="30"/>
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="37"/>
     </row>
     <row r="4" spans="2:19" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="35"/>
-      <c r="C4" s="17" t="s">
+      <c r="B4" s="36"/>
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="18" t="s">
+      <c r="J4" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="K4" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="18" t="s">
+      <c r="L4" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="18" t="s">
+      <c r="M4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="N4" s="18" t="s">
+      <c r="N4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="O4" s="18" t="s">
+      <c r="O4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="Q4" s="18" t="s">
+      <c r="Q4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="S4" s="36"/>
+      <c r="S4" s="37"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B5" s="35"/>
-      <c r="C5" s="30" t="s">
+      <c r="B5" s="36"/>
+      <c r="C5" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="30" t="s">
+      <c r="D5" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="30" t="s">
+      <c r="E5" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G5" s="30" t="s">
+      <c r="G5" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="30" t="s">
+      <c r="H5" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="I5" s="31">
+      <c r="I5" s="32">
         <v>437273953</v>
       </c>
-      <c r="J5" s="30">
+      <c r="J5" s="31">
         <v>376</v>
       </c>
-      <c r="K5" s="31">
+      <c r="K5" s="32">
         <v>14850352</v>
       </c>
-      <c r="L5" s="30">
+      <c r="L5" s="31">
         <v>13</v>
       </c>
-      <c r="M5" s="31">
+      <c r="M5" s="32">
         <v>1850</v>
       </c>
-      <c r="N5" s="31">
+      <c r="N5" s="32">
         <v>412669</v>
       </c>
-      <c r="O5" s="30">
+      <c r="O5" s="31">
         <v>267</v>
       </c>
-      <c r="P5" s="30">
+      <c r="P5" s="31">
         <v>26</v>
       </c>
-      <c r="Q5" s="30">
+      <c r="Q5" s="31">
         <v>376</v>
       </c>
-      <c r="R5" s="30"/>
-      <c r="S5" s="36"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="37"/>
     </row>
     <row r="6" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="35"/>
-      <c r="C6" s="30" t="s">
+      <c r="B6" s="36"/>
+      <c r="C6" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="30" t="s">
+      <c r="E6" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="30" t="s">
+      <c r="H6" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="I6" s="31">
+      <c r="I6" s="32">
         <v>471985164</v>
       </c>
-      <c r="J6" s="30">
+      <c r="J6" s="31">
         <v>548</v>
       </c>
-      <c r="K6" s="31">
+      <c r="K6" s="32">
         <v>12200365</v>
       </c>
-      <c r="L6" s="30">
+      <c r="L6" s="31">
         <v>15</v>
       </c>
-      <c r="M6" s="31">
+      <c r="M6" s="32">
         <v>2127</v>
       </c>
-      <c r="N6" s="31">
+      <c r="N6" s="32">
         <v>347532</v>
       </c>
-      <c r="O6" s="30">
+      <c r="O6" s="31">
         <v>333</v>
       </c>
-      <c r="P6" s="30">
+      <c r="P6" s="31">
         <v>26</v>
       </c>
-      <c r="Q6" s="30">
+      <c r="Q6" s="31">
         <v>548</v>
       </c>
-      <c r="R6" s="30"/>
-      <c r="S6" s="36"/>
+      <c r="R6" s="31"/>
+      <c r="S6" s="37"/>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B7" s="35"/>
-      <c r="C7" s="30" t="s">
+      <c r="B7" s="36"/>
+      <c r="C7" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="I7" s="31">
+      <c r="I7" s="32">
         <v>416131685</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="32">
         <v>324311</v>
       </c>
-      <c r="K7" s="31">
+      <c r="K7" s="32">
         <v>3050</v>
       </c>
-      <c r="L7" s="31">
+      <c r="L7" s="32">
         <v>34112</v>
       </c>
-      <c r="M7" s="31">
+      <c r="M7" s="32">
         <v>330739</v>
       </c>
-      <c r="N7" s="31">
+      <c r="N7" s="32">
         <v>2918</v>
       </c>
-      <c r="O7" s="31">
+      <c r="O7" s="32">
         <v>35367</v>
       </c>
-      <c r="P7" s="30">
+      <c r="P7" s="31">
         <v>0</v>
       </c>
-      <c r="Q7" s="30">
+      <c r="Q7" s="31">
         <v>324311</v>
       </c>
-      <c r="R7" s="31"/>
-      <c r="S7" s="36"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="37"/>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B8" s="35"/>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="36"/>
+      <c r="C8" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="30" t="s">
+      <c r="D8" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="31" t="s">
         <v>35</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="30" t="s">
+      <c r="H8" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="I8" s="31">
+      <c r="I8" s="32">
         <v>342758722</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="32">
         <v>73274</v>
       </c>
-      <c r="K8" s="31">
+      <c r="K8" s="32">
         <v>6820</v>
       </c>
-      <c r="L8" s="31">
+      <c r="L8" s="32">
         <v>13139</v>
       </c>
-      <c r="M8" s="31">
+      <c r="M8" s="32">
         <v>99348</v>
       </c>
-      <c r="N8" s="31">
+      <c r="N8" s="32">
         <v>4524</v>
       </c>
-      <c r="O8" s="31">
+      <c r="O8" s="32">
         <v>21105</v>
       </c>
-      <c r="P8" s="30">
+      <c r="P8" s="31">
         <v>0</v>
       </c>
-      <c r="Q8" s="30">
+      <c r="Q8" s="31">
         <v>73274</v>
       </c>
-      <c r="R8" s="31"/>
-      <c r="S8" s="36"/>
+      <c r="R8" s="32"/>
+      <c r="S8" s="37"/>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="30" t="s">
+      <c r="B9" s="36"/>
+      <c r="C9" s="31" t="s">
         <v>115</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="G9" s="30" t="s">
+      <c r="G9" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="H9" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="I9" s="31">
+      <c r="I9" s="32">
         <v>34375595</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="32">
         <v>460000</v>
       </c>
-      <c r="L9" s="30">
+      <c r="L9" s="31">
         <v>477</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="32">
         <v>20639</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="32">
         <v>2124</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="32">
         <v>4887</v>
       </c>
-      <c r="P9" s="30">
+      <c r="P9" s="31">
         <v>0</v>
       </c>
-      <c r="Q9" s="30">
+      <c r="Q9" s="31">
         <v>20639</v>
       </c>
-      <c r="R9" s="31"/>
-      <c r="S9" s="36"/>
+      <c r="R9" s="32"/>
+      <c r="S9" s="37"/>
     </row>
     <row r="10" spans="2:19" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="37"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="38"/>
-      <c r="H10" s="38"/>
-      <c r="I10" s="38"/>
-      <c r="J10" s="38"/>
-      <c r="K10" s="38"/>
-      <c r="L10" s="38"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="38"/>
-      <c r="O10" s="38"/>
-      <c r="P10" s="38"/>
-      <c r="Q10" s="38"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="39"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
+      <c r="G10" s="39"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="39"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="39"/>
+      <c r="O10" s="39"/>
+      <c r="P10" s="39"/>
+      <c r="Q10" s="39"/>
+      <c r="R10" s="39"/>
+      <c r="S10" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2487,245 +2622,245 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="2" width="2.5" style="13" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="13"/>
-    <col min="4" max="4" width="11.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="12" style="13" customWidth="1"/>
-    <col min="10" max="10" width="10.83203125" style="13"/>
-    <col min="11" max="11" width="2.33203125" style="13" customWidth="1"/>
-    <col min="12" max="14" width="10.83203125" style="13"/>
-    <col min="15" max="15" width="29.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.83203125" style="13" customWidth="1"/>
-    <col min="17" max="17" width="31.6640625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="32.5" style="13" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="2.5" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="11.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="12" style="14" customWidth="1"/>
+    <col min="10" max="10" width="10.83203125" style="14"/>
+    <col min="11" max="11" width="2.33203125" style="14" customWidth="1"/>
+    <col min="12" max="14" width="10.83203125" style="14"/>
+    <col min="15" max="15" width="29.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" style="14" customWidth="1"/>
+    <col min="17" max="17" width="31.6640625" style="14" customWidth="1"/>
+    <col min="18" max="18" width="32.5" style="14" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="43"/>
     </row>
     <row r="3" spans="2:18" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="43"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="44"/>
+      <c r="C3" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
-      <c r="I3" s="44"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="46"/>
     </row>
     <row r="4" spans="2:18" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="43"/>
-      <c r="C4" s="46" t="s">
+      <c r="B4" s="44"/>
+      <c r="C4" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="46" t="s">
+      <c r="D4" s="47" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="46" t="s">
+      <c r="F4" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="47" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="46" t="s">
+      <c r="H4" s="47" t="s">
         <v>141</v>
       </c>
-      <c r="I4" s="46" t="s">
+      <c r="I4" s="47" t="s">
         <v>123</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="47" t="s">
         <v>142</v>
       </c>
-      <c r="K4" s="45"/>
+      <c r="K4" s="46"/>
     </row>
     <row r="5" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="43"/>
-      <c r="C5" s="47" t="s">
+      <c r="B5" s="44"/>
+      <c r="C5" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="48" t="s">
+      <c r="D5" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="E5" s="48" t="s">
+      <c r="E5" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G5" s="48" t="s">
+      <c r="G5" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H5" s="48"/>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48"/>
-      <c r="K5" s="45"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="46"/>
     </row>
     <row r="6" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="43"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48" t="s">
+      <c r="B6" s="44"/>
+      <c r="C6" s="48"/>
+      <c r="D6" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="48" t="s">
+      <c r="F6" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G6" s="48" t="s">
+      <c r="G6" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="H6" s="48"/>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48" t="s">
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="K6" s="45"/>
+      <c r="K6" s="46"/>
     </row>
     <row r="7" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="43"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48" t="s">
+      <c r="B7" s="44"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H7" s="48"/>
-      <c r="I7" s="48"/>
-      <c r="J7" s="48"/>
-      <c r="K7" s="45"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
+      <c r="K7" s="46"/>
     </row>
     <row r="8" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="43"/>
-      <c r="C8" s="47" t="s">
+      <c r="B8" s="44"/>
+      <c r="C8" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="E8" s="48" t="s">
+      <c r="E8" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F8" s="48" t="s">
+      <c r="F8" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G8" s="48" t="s">
+      <c r="G8" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="45"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="46"/>
     </row>
     <row r="9" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="43"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="48"/>
+      <c r="D9" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="E9" s="48" t="s">
+      <c r="E9" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="48" t="s">
+      <c r="F9" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="45"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="46"/>
     </row>
     <row r="10" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="43"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="48" t="s">
+      <c r="B10" s="44"/>
+      <c r="C10" s="48"/>
+      <c r="D10" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="E10" s="48" t="s">
+      <c r="E10" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F10" s="48" t="s">
+      <c r="F10" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="45"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="46"/>
     </row>
     <row r="11" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="43"/>
-      <c r="C11" s="47" t="s">
+      <c r="B11" s="44"/>
+      <c r="C11" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="48" t="s">
+      <c r="D11" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="E11" s="48" t="s">
+      <c r="E11" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="48" t="s">
+      <c r="F11" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G11" s="48" t="s">
+      <c r="G11" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H11" s="48"/>
-      <c r="I11" s="48"/>
-      <c r="J11" s="48"/>
-      <c r="K11" s="45"/>
+      <c r="H11" s="49"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="46"/>
     </row>
     <row r="12" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="43"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="48" t="s">
+      <c r="B12" s="44"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="48" t="s">
+      <c r="E12" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="48" t="s">
+      <c r="F12" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G12" s="48" t="s">
+      <c r="G12" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H12" s="48"/>
-      <c r="I12" s="48"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="45"/>
-      <c r="O12" s="52" t="s">
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="46"/>
+      <c r="O12" s="53" t="s">
         <v>119</v>
       </c>
       <c r="P12"/>
@@ -2733,25 +2868,25 @@
       <c r="R12"/>
     </row>
     <row r="13" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="43"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="48" t="s">
+      <c r="B13" s="44"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="48" t="s">
+      <c r="E13" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="48" t="s">
+      <c r="F13" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G13" s="48" t="s">
+      <c r="G13" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="48"/>
-      <c r="J13" s="48"/>
-      <c r="K13" s="45"/>
-      <c r="O13" s="52" t="s">
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="46"/>
+      <c r="O13" s="53" t="s">
         <v>120</v>
       </c>
       <c r="P13"/>
@@ -2759,447 +2894,447 @@
       <c r="R13"/>
     </row>
     <row r="14" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="43"/>
-      <c r="C14" s="47" t="s">
+      <c r="B14" s="44"/>
+      <c r="C14" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="48" t="s">
+      <c r="D14" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="48" t="s">
+      <c r="E14" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F14" s="48" t="s">
+      <c r="F14" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="G14" s="48" t="s">
+      <c r="G14" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="48"/>
-      <c r="K14" s="45"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="46"/>
       <c r="O14"/>
       <c r="P14"/>
       <c r="Q14"/>
       <c r="R14"/>
     </row>
     <row r="15" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="43"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="48" t="s">
+      <c r="B15" s="44"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="48" t="s">
+      <c r="E15" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="48" t="s">
+      <c r="F15" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="48" t="s">
+      <c r="G15" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H15" s="48"/>
-      <c r="I15" s="48"/>
-      <c r="J15" s="48"/>
-      <c r="K15" s="45"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="46"/>
       <c r="O15"/>
       <c r="P15"/>
       <c r="Q15"/>
       <c r="R15"/>
     </row>
     <row r="16" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="43"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="48" t="s">
+      <c r="B16" s="44"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="48" t="s">
+      <c r="E16" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="F16" s="48" t="s">
+      <c r="F16" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G16" s="48" t="s">
+      <c r="G16" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="45"/>
-      <c r="O16" s="53" t="s">
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="46"/>
+      <c r="O16" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="P16" s="54" t="s">
+      <c r="P16" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="Q16" s="54" t="s">
+      <c r="Q16" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="R16" s="54" t="s">
+      <c r="R16" s="55" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="43"/>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48" t="s">
+      <c r="B17" s="44"/>
+      <c r="C17" s="48"/>
+      <c r="D17" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="48" t="s">
+      <c r="E17" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="F17" s="48" t="s">
+      <c r="F17" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G17" s="48" t="s">
+      <c r="G17" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
-      <c r="J17" s="48"/>
-      <c r="K17" s="45"/>
-      <c r="O17" s="53"/>
-      <c r="P17" s="53"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="46"/>
+      <c r="O17" s="54"/>
+      <c r="P17" s="54"/>
+      <c r="Q17" s="54"/>
+      <c r="R17" s="54"/>
     </row>
     <row r="18" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="43"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48" t="s">
+      <c r="B18" s="44"/>
+      <c r="C18" s="48"/>
+      <c r="D18" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="48" t="s">
+      <c r="E18" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="48" t="s">
+      <c r="F18" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="G18" s="48" t="s">
+      <c r="G18" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="45"/>
-      <c r="O18" s="53" t="s">
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="46"/>
+      <c r="O18" s="54" t="s">
         <v>125</v>
       </c>
-      <c r="P18" s="53">
+      <c r="P18" s="54">
         <v>1.87</v>
       </c>
-      <c r="Q18" s="53">
+      <c r="Q18" s="54">
         <v>1.76</v>
       </c>
-      <c r="R18" s="53" t="s">
+      <c r="R18" s="54" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="43"/>
-      <c r="C19" s="47"/>
-      <c r="D19" s="48" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="E19" s="48" t="s">
+      <c r="E19" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F19" s="48" t="s">
+      <c r="F19" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G19" s="48" t="s">
+      <c r="G19" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="45"/>
-      <c r="O19" s="53" t="s">
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="46"/>
+      <c r="O19" s="54" t="s">
         <v>127</v>
       </c>
-      <c r="P19" s="53">
+      <c r="P19" s="54">
         <v>1.88</v>
       </c>
-      <c r="Q19" s="53">
+      <c r="Q19" s="54">
         <v>1.53</v>
       </c>
-      <c r="R19" s="53" t="s">
+      <c r="R19" s="54" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="43"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48" t="s">
+      <c r="B20" s="44"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="E20" s="48" t="s">
+      <c r="E20" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="48" t="s">
+      <c r="F20" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G20" s="48" t="s">
+      <c r="G20" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H20" s="48"/>
-      <c r="I20" s="48"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="45"/>
-      <c r="O20" s="53" t="s">
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="46"/>
+      <c r="O20" s="54" t="s">
         <v>129</v>
       </c>
-      <c r="P20" s="53">
+      <c r="P20" s="54">
         <v>1.73</v>
       </c>
-      <c r="Q20" s="53">
+      <c r="Q20" s="54">
         <v>1.3</v>
       </c>
-      <c r="R20" s="53" t="s">
+      <c r="R20" s="54" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="43"/>
-      <c r="C21" s="47"/>
-      <c r="D21" s="48" t="s">
+      <c r="B21" s="44"/>
+      <c r="C21" s="48"/>
+      <c r="D21" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="H21" s="48"/>
-      <c r="I21" s="48"/>
-      <c r="J21" s="48" t="s">
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="K21" s="45"/>
-      <c r="O21" s="53" t="s">
+      <c r="K21" s="46"/>
+      <c r="O21" s="54" t="s">
         <v>131</v>
       </c>
-      <c r="P21" s="53">
+      <c r="P21" s="54">
         <v>1</v>
       </c>
-      <c r="Q21" s="53">
+      <c r="Q21" s="54">
         <v>1.33</v>
       </c>
-      <c r="R21" s="53" t="s">
+      <c r="R21" s="54" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="43"/>
-      <c r="C22" s="47" t="s">
+      <c r="B22" s="44"/>
+      <c r="C22" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D22" s="48" t="s">
+      <c r="D22" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="48" t="s">
+      <c r="E22" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F22" s="48" t="s">
+      <c r="F22" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="G22" s="48" t="s">
+      <c r="G22" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="45"/>
-      <c r="O22" s="53" t="s">
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="46"/>
+      <c r="O22" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="P22" s="53">
+      <c r="P22" s="54">
         <v>1.84</v>
       </c>
-      <c r="Q22" s="53">
+      <c r="Q22" s="54">
         <v>2.2200000000000002</v>
       </c>
-      <c r="R22" s="53" t="s">
+      <c r="R22" s="54" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="43"/>
-      <c r="C23" s="47"/>
-      <c r="D23" s="48" t="s">
+      <c r="B23" s="44"/>
+      <c r="C23" s="48"/>
+      <c r="D23" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="48" t="s">
+      <c r="E23" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="48" t="s">
+      <c r="F23" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G23" s="48" t="s">
+      <c r="G23" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H23" s="48"/>
-      <c r="I23" s="48"/>
-      <c r="J23" s="48"/>
-      <c r="K23" s="45"/>
-      <c r="O23" s="53" t="s">
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="46"/>
+      <c r="O23" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="P23" s="53">
+      <c r="P23" s="54">
         <v>1.26</v>
       </c>
-      <c r="Q23" s="53">
+      <c r="Q23" s="54">
         <v>1.52</v>
       </c>
-      <c r="R23" s="53" t="s">
+      <c r="R23" s="54" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="43"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="48" t="s">
+      <c r="B24" s="44"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="E24" s="48" t="s">
+      <c r="E24" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="48" t="s">
+      <c r="F24" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G24" s="48" t="s">
+      <c r="G24" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="48"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="45"/>
-      <c r="O24" s="53" t="s">
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="46"/>
+      <c r="O24" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="P24" s="53">
+      <c r="P24" s="54">
         <v>1.84</v>
       </c>
-      <c r="Q24" s="53">
+      <c r="Q24" s="54">
         <v>1.8</v>
       </c>
-      <c r="R24" s="53" t="s">
+      <c r="R24" s="54" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="25" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="43"/>
-      <c r="C25" s="47"/>
-      <c r="D25" s="48" t="s">
+      <c r="B25" s="44"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="E25" s="48" t="s">
+      <c r="E25" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="G25" s="48" t="s">
+      <c r="G25" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H25" s="48"/>
-      <c r="I25" s="48"/>
-      <c r="J25" s="48"/>
-      <c r="K25" s="45"/>
-      <c r="O25" s="53" t="s">
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="46"/>
+      <c r="O25" s="54" t="s">
         <v>138</v>
       </c>
-      <c r="P25" s="53">
+      <c r="P25" s="54">
         <v>1.91</v>
       </c>
-      <c r="Q25" s="53">
+      <c r="Q25" s="54">
         <v>2.02</v>
       </c>
-      <c r="R25" s="53" t="s">
+      <c r="R25" s="54" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="43"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="48" t="s">
+      <c r="B26" s="44"/>
+      <c r="C26" s="48"/>
+      <c r="D26" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="48" t="s">
+      <c r="E26" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F26" s="48" t="s">
+      <c r="F26" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G26" s="48" t="s">
+      <c r="G26" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="49">
         <v>1.91</v>
       </c>
-      <c r="I26" s="48">
+      <c r="I26" s="49">
         <v>2.02</v>
       </c>
-      <c r="J26" s="48" t="s">
+      <c r="J26" s="49" t="s">
         <v>128</v>
       </c>
-      <c r="K26" s="45"/>
+      <c r="K26" s="46"/>
       <c r="O26"/>
       <c r="P26"/>
       <c r="Q26"/>
       <c r="R26"/>
     </row>
     <row r="27" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="43"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="48" t="s">
+      <c r="B27" s="44"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="E27" s="48" t="s">
+      <c r="E27" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G27" s="48" t="s">
+      <c r="G27" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="48"/>
-      <c r="I27" s="48"/>
-      <c r="J27" s="48"/>
-      <c r="K27" s="45"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="46"/>
       <c r="O27"/>
       <c r="P27"/>
       <c r="Q27"/>
       <c r="R27"/>
     </row>
     <row r="28" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="43"/>
-      <c r="C28" s="47" t="s">
+      <c r="B28" s="44"/>
+      <c r="C28" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="D28" s="48" t="s">
+      <c r="D28" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="E28" s="48" t="s">
+      <c r="E28" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G28" s="48" t="s">
+      <c r="G28" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="48"/>
-      <c r="I28" s="48"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="45"/>
-      <c r="O28" s="53" t="s">
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="46"/>
+      <c r="O28" s="54" t="s">
         <v>139</v>
       </c>
       <c r="P28"/>
@@ -3207,27 +3342,27 @@
       <c r="R28"/>
     </row>
     <row r="29" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B29" s="43"/>
-      <c r="C29" s="47"/>
-      <c r="D29" s="48" t="s">
+      <c r="B29" s="44"/>
+      <c r="C29" s="48"/>
+      <c r="D29" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="48"/>
-      <c r="I29" s="48"/>
-      <c r="J29" s="48" t="s">
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49" t="s">
         <v>152</v>
       </c>
-      <c r="K29" s="45"/>
-      <c r="O29" s="53" t="s">
+      <c r="K29" s="46"/>
+      <c r="O29" s="54" t="s">
         <v>140</v>
       </c>
       <c r="P29"/>
@@ -3235,36 +3370,36 @@
       <c r="R29"/>
     </row>
     <row r="30" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="43"/>
-      <c r="C30" s="47"/>
-      <c r="D30" s="48" t="s">
+      <c r="B30" s="44"/>
+      <c r="C30" s="48"/>
+      <c r="D30" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="E30" s="48" t="s">
+      <c r="E30" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="G30" s="48" t="s">
+      <c r="G30" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="H30" s="48"/>
-      <c r="I30" s="48"/>
-      <c r="J30" s="48"/>
-      <c r="K30" s="45"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="46"/>
     </row>
     <row r="31" spans="2:18" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="49"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="50"/>
-      <c r="K31" s="51"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
+      <c r="K31" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -3290,130 +3425,130 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="F3" s="23" t="s">
+      <c r="F3" s="24" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="26">
         <v>1</v>
       </c>
-      <c r="F4" s="26">
+      <c r="F4" s="27">
         <v>67</v>
       </c>
     </row>
     <row r="5" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="26">
         <v>1</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="27">
         <v>97</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="26">
         <v>2</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="27">
         <v>35</v>
       </c>
     </row>
     <row r="7" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="26" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="26">
         <v>3</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="27">
         <v>29</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="26">
         <v>1</v>
       </c>
-      <c r="F8" s="26" t="s">
+      <c r="F8" s="27" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="26">
         <v>1</v>
       </c>
-      <c r="F9" s="26" t="s">
+      <c r="F9" s="27" t="s">
         <v>107</v>
       </c>
     </row>
@@ -3432,419 +3567,419 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="2" width="3.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="13" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.83203125" style="13" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="13" customWidth="1"/>
-    <col min="9" max="9" width="16.5" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="16.5" style="13" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="13"/>
-    <col min="14" max="14" width="11.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="3.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="14" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="16.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.5" style="14" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="14"/>
+    <col min="14" max="14" width="11.83203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="28" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="28" t="s">
         <v>145</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="28" t="s">
         <v>144</v>
       </c>
-      <c r="H3" s="27" t="s">
+      <c r="H3" s="28" t="s">
         <v>143</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="I3" s="28" t="s">
         <v>146</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="L3" s="27" t="s">
+      <c r="L3" s="28" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="17">
         <v>7790139515</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="17">
         <v>7617422156</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G4" s="17">
         <v>6484</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="17">
         <v>1275836</v>
       </c>
-      <c r="I4" s="16">
+      <c r="I4" s="17">
         <v>5970</v>
       </c>
-      <c r="J4" s="55">
+      <c r="J4" s="56">
         <v>0.44755</v>
       </c>
-      <c r="K4" s="55"/>
-      <c r="L4" s="15" t="s">
+      <c r="K4" s="56"/>
+      <c r="L4" s="16" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="17">
         <v>6534076057</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="17">
         <v>6404937329</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G5" s="17">
         <v>14390</v>
       </c>
-      <c r="H5" s="16">
+      <c r="H5" s="17">
         <v>624944</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="17">
         <v>10248</v>
       </c>
-      <c r="J5" s="55">
+      <c r="J5" s="56">
         <v>0.45040000000000002</v>
       </c>
-      <c r="K5" s="55"/>
-      <c r="L5" s="15" t="s">
+      <c r="K5" s="56"/>
+      <c r="L5" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="E6" s="16">
+      <c r="E6" s="17">
         <v>14225369483</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="17">
         <v>13962511851</v>
       </c>
-      <c r="G6" s="16">
+      <c r="G6" s="17">
         <v>16557</v>
       </c>
-      <c r="H6" s="16">
+      <c r="H6" s="17">
         <v>840724</v>
       </c>
-      <c r="I6" s="16">
+      <c r="I6" s="17">
         <v>16607</v>
       </c>
-      <c r="J6" s="55">
+      <c r="J6" s="56">
         <v>0.44650000000000001</v>
       </c>
-      <c r="K6" s="55"/>
-      <c r="L6" s="15" t="s">
+      <c r="K6" s="56"/>
+      <c r="L6" s="16" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E7" s="16">
+      <c r="E7" s="17">
         <v>24466806025</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="17">
         <v>23993220246</v>
       </c>
-      <c r="G7" s="15"/>
-      <c r="H7" s="16">
+      <c r="G7" s="16"/>
+      <c r="H7" s="17">
         <v>2054534</v>
       </c>
-      <c r="I7" s="16">
+      <c r="I7" s="17">
         <v>11678</v>
       </c>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-      <c r="L7" s="15" t="s">
+      <c r="J7" s="56"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="16" t="s">
         <v>104</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E8" s="17">
         <v>11375170745</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="17">
         <v>11151984598</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G8" s="17">
         <v>11420</v>
       </c>
-      <c r="H8" s="16">
+      <c r="H8" s="17">
         <v>1040599</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I8" s="17">
         <v>10716</v>
       </c>
-      <c r="J8" s="55">
+      <c r="J8" s="56">
         <v>0.44180000000000003</v>
       </c>
-      <c r="K8" s="55"/>
-      <c r="L8" s="15" t="s">
+      <c r="K8" s="56"/>
+      <c r="L8" s="16" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16">
+      <c r="E9" s="16"/>
+      <c r="F9" s="17">
         <v>94825601818</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16">
+      <c r="G9" s="16"/>
+      <c r="H9" s="17">
         <v>627984118</v>
       </c>
-      <c r="I9" s="15">
+      <c r="I9" s="16">
         <v>151</v>
       </c>
-      <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="15">
+      <c r="J9" s="56"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="16">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="D10" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="15"/>
-      <c r="F10" s="16">
+      <c r="E10" s="16"/>
+      <c r="F10" s="17">
         <v>94825601818</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16">
+      <c r="G10" s="16"/>
+      <c r="H10" s="17">
         <v>627984118</v>
       </c>
-      <c r="I10" s="15">
+      <c r="I10" s="16">
         <v>151</v>
       </c>
-      <c r="J10" s="55"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="15">
+      <c r="J10" s="56"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="16">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="17">
         <v>161450851775</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="17">
         <v>65806680934</v>
       </c>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16">
+      <c r="G11" s="16"/>
+      <c r="H11" s="17">
         <v>435805834</v>
       </c>
-      <c r="I11" s="15">
+      <c r="I11" s="16">
         <v>151</v>
       </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="15">
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="16">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E12" s="17">
         <v>161450851775</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="17">
         <v>65806680934</v>
       </c>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16">
+      <c r="G12" s="16"/>
+      <c r="H12" s="17">
         <v>435805834</v>
       </c>
-      <c r="I12" s="15">
+      <c r="I12" s="16">
         <v>151</v>
       </c>
-      <c r="J12" s="55"/>
-      <c r="K12" s="55"/>
-      <c r="L12" s="15">
+      <c r="J12" s="56"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="16">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E18" s="13">
+      <c r="E18" s="14">
         <v>1200000000</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="14">
         <v>490000000</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="14" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="19" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E19" s="13">
+      <c r="E19" s="14">
         <f>F9/E18</f>
         <v>79.021334848333339</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="14">
         <f>(F10/F18)/2</f>
         <v>96.760818181632658</v>
       </c>
-      <c r="G19" s="13" t="s">
+      <c r="G19" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H19" s="15">
         <f>SUM(F4:F6)</f>
         <v>27984871336</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="14">
         <f>(H19/490000000)/2</f>
         <v>28.555991159183673</v>
       </c>
-      <c r="K19" s="14">
+      <c r="K19" s="15">
         <f>SUM(H4:H6)</f>
         <v>2741504</v>
       </c>
-      <c r="L19" s="13">
+      <c r="L19" s="14">
         <v>2741504</v>
       </c>
     </row>
     <row r="20" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E20" s="13">
+      <c r="E20" s="14">
         <f>F11/E18</f>
         <v>54.838900778333333</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="14">
         <f>(F11/F18)/2</f>
         <v>67.149674422448982</v>
       </c>
-      <c r="G20" s="13" t="s">
+      <c r="G20" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="14">
+      <c r="H20" s="15">
         <f>SUM(E7:E8)</f>
         <v>35841976770</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="14">
         <f>(H20/490000000)/2</f>
         <v>36.573445683673469</v>
       </c>
-      <c r="K20" s="14">
+      <c r="K20" s="15">
         <f>SUM(H7:H8)</f>
         <v>3095133</v>
       </c>
-      <c r="L20" s="13">
+      <c r="L20" s="14">
         <v>3095133</v>
       </c>
     </row>
     <row r="23" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="H23" s="13">
+      <c r="H23" s="14">
         <v>27984871336</v>
       </c>
     </row>
     <row r="24" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="H24" s="13">
+      <c r="H24" s="14">
         <v>35841976770</v>
       </c>
     </row>
@@ -3858,393 +3993,457 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF36CC-2E6B-0D43-87A8-02414AEC4EB5}">
-  <dimension ref="B3:P13"/>
+  <dimension ref="C2:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="13"/>
-    <col min="2" max="2" width="14.1640625" style="13" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="13"/>
-    <col min="4" max="4" width="13.6640625" style="13" customWidth="1"/>
-    <col min="5" max="7" width="11.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="11.1640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="13"/>
+    <col min="1" max="1" width="10.83203125" style="14"/>
+    <col min="2" max="2" width="2.6640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="14.1640625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="14"/>
+    <col min="5" max="5" width="13.6640625" style="14" customWidth="1"/>
+    <col min="6" max="8" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" style="14" customWidth="1"/>
+    <col min="15" max="15" width="2.83203125" style="14" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="86" t="s">
-        <v>170</v>
-      </c>
-      <c r="C3" s="86"/>
-      <c r="D3" s="86"/>
-      <c r="E3" s="86"/>
-      <c r="F3" s="86"/>
-      <c r="G3" s="86"/>
-      <c r="H3" s="86"/>
-      <c r="I3" s="86"/>
-      <c r="J3" s="86"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="P3" s="89"/>
-    </row>
-    <row r="4" spans="2:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="56" t="s">
+    <row r="2" spans="3:17" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="3:17" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="D3" s="81"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="81"/>
+      <c r="G3" s="81"/>
+      <c r="H3" s="81"/>
+      <c r="I3" s="81"/>
+      <c r="J3" s="81"/>
+      <c r="K3" s="81"/>
+      <c r="L3" s="81"/>
+      <c r="M3" s="81"/>
+      <c r="N3" s="81"/>
+      <c r="Q3" s="84"/>
+    </row>
+    <row r="4" spans="3:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C4" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="D4" s="86"/>
+      <c r="E4" s="58" t="s">
         <v>154</v>
       </c>
-      <c r="E4" s="59"/>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="58" t="s">
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="88" t="s">
         <v>155</v>
       </c>
-      <c r="J4" s="59"/>
       <c r="K4" s="59"/>
       <c r="L4" s="59"/>
-      <c r="M4" s="60"/>
-    </row>
-    <row r="5" spans="2:16" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="61"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="63" t="s">
+      <c r="M4" s="59"/>
+      <c r="N4" s="60"/>
+    </row>
+    <row r="5" spans="3:17" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="61"/>
+      <c r="D5" s="85"/>
+      <c r="E5" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="89" t="s">
+        <v>167</v>
+      </c>
+      <c r="G5" s="89" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="89" t="s">
         <v>169</v>
       </c>
-      <c r="E5" s="64" t="s">
+      <c r="I5" s="90" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" s="89" t="s">
+        <v>167</v>
+      </c>
+      <c r="L5" s="89" t="s">
+        <v>168</v>
+      </c>
+      <c r="M5" s="89" t="s">
+        <v>169</v>
+      </c>
+      <c r="N5" s="90" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="3:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C6" s="62" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="63" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6" s="64">
+        <v>11604</v>
+      </c>
+      <c r="F6" s="65">
+        <v>353581</v>
+      </c>
+      <c r="G6" s="65">
+        <v>1188596</v>
+      </c>
+      <c r="H6" s="65">
+        <v>2749144</v>
+      </c>
+      <c r="I6" s="66">
+        <v>12200365</v>
+      </c>
+      <c r="J6" s="64">
+        <v>15048</v>
+      </c>
+      <c r="K6" s="65">
+        <v>418614</v>
+      </c>
+      <c r="L6" s="65">
+        <v>1392224</v>
+      </c>
+      <c r="M6" s="65">
+        <v>4383157</v>
+      </c>
+      <c r="N6" s="66">
+        <v>14850352</v>
+      </c>
+    </row>
+    <row r="7" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="C7" s="67"/>
+      <c r="D7" s="68" t="s">
         <v>156</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="E7" s="70">
+        <v>1276120</v>
+      </c>
+      <c r="F7" s="69">
+        <v>324</v>
+      </c>
+      <c r="G7" s="69">
+        <v>106</v>
+      </c>
+      <c r="H7" s="69">
+        <v>38</v>
+      </c>
+      <c r="I7" s="68">
+        <v>15</v>
+      </c>
+      <c r="J7" s="70">
+        <v>771808</v>
+      </c>
+      <c r="K7" s="69">
+        <v>264</v>
+      </c>
+      <c r="L7" s="69">
+        <v>80</v>
+      </c>
+      <c r="M7" s="69">
+        <v>26</v>
+      </c>
+      <c r="N7" s="68">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="C8" s="67"/>
+      <c r="D8" s="68" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="83">
+        <v>3095133</v>
+      </c>
+      <c r="F8" s="69">
+        <v>2086</v>
+      </c>
+      <c r="G8" s="69">
+        <v>1106</v>
+      </c>
+      <c r="H8" s="69">
+        <v>705</v>
+      </c>
+      <c r="I8" s="68">
+        <v>549</v>
+      </c>
+      <c r="J8" s="83">
+        <v>2741504</v>
+      </c>
+      <c r="K8" s="69">
+        <v>1805</v>
+      </c>
+      <c r="L8" s="69">
+        <v>1012</v>
+      </c>
+      <c r="M8" s="69">
+        <v>515</v>
+      </c>
+      <c r="N8" s="68">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="9" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="C9" s="67"/>
+      <c r="D9" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="G5" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="H5" s="65" t="s">
-        <v>166</v>
-      </c>
-      <c r="I5" s="63" t="s">
-        <v>169</v>
-      </c>
-      <c r="J5" s="64" t="s">
-        <v>156</v>
-      </c>
-      <c r="K5" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="L5" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="M5" s="65" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="66" t="s">
-        <v>167</v>
-      </c>
-      <c r="C6" s="67" t="s">
-        <v>144</v>
-      </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="69">
-        <v>353581</v>
-      </c>
-      <c r="F6" s="69">
-        <v>1188596</v>
-      </c>
-      <c r="G6" s="69">
-        <v>2749144</v>
-      </c>
-      <c r="H6" s="70">
-        <v>12200365</v>
-      </c>
-      <c r="I6" s="68">
-        <v>15048</v>
-      </c>
-      <c r="J6" s="69">
-        <v>418614</v>
-      </c>
-      <c r="K6" s="69">
-        <v>1392224</v>
-      </c>
-      <c r="L6" s="69">
-        <v>4383157</v>
-      </c>
-      <c r="M6" s="70">
-        <v>14850352</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B7" s="71"/>
-      <c r="C7" s="72" t="s">
-        <v>157</v>
-      </c>
-      <c r="D7" s="73"/>
-      <c r="E7" s="74">
-        <v>324</v>
-      </c>
-      <c r="F7" s="74">
-        <v>106</v>
-      </c>
-      <c r="G7" s="74">
-        <v>38</v>
-      </c>
-      <c r="H7" s="72">
-        <v>15</v>
-      </c>
-      <c r="I7" s="75">
-        <v>771808</v>
-      </c>
-      <c r="J7" s="74">
-        <v>264</v>
-      </c>
-      <c r="K7" s="74">
-        <v>80</v>
-      </c>
-      <c r="L7" s="74">
-        <v>26</v>
-      </c>
-      <c r="M7" s="72">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B8" s="71"/>
-      <c r="C8" s="72" t="s">
+      <c r="E9" s="82">
+        <v>35145204844</v>
+      </c>
+      <c r="F9" s="71">
+        <v>471831811</v>
+      </c>
+      <c r="G9" s="71">
+        <v>471929811</v>
+      </c>
+      <c r="H9" s="71">
+        <v>472145811</v>
+      </c>
+      <c r="I9" s="72">
+        <v>472157411</v>
+      </c>
+      <c r="J9" s="82">
+        <v>27984871336</v>
+      </c>
+      <c r="K9" s="71">
+        <v>436920153</v>
+      </c>
+      <c r="L9" s="71">
+        <v>436999453</v>
+      </c>
+      <c r="M9" s="71">
+        <v>437264453</v>
+      </c>
+      <c r="N9" s="72">
+        <v>437273953</v>
+      </c>
+    </row>
+    <row r="10" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="67" t="s">
         <v>158</v>
       </c>
-      <c r="D8" s="88">
-        <v>3095133</v>
-      </c>
-      <c r="E8" s="74">
-        <v>2086</v>
-      </c>
-      <c r="F8" s="74">
-        <v>1106</v>
-      </c>
-      <c r="G8" s="74">
-        <v>705</v>
-      </c>
-      <c r="H8" s="72">
-        <v>549</v>
-      </c>
-      <c r="I8" s="88">
-        <v>2741504</v>
-      </c>
-      <c r="J8" s="74">
-        <v>1805</v>
-      </c>
-      <c r="K8" s="74">
-        <v>1012</v>
-      </c>
-      <c r="L8" s="74">
-        <v>515</v>
-      </c>
-      <c r="M8" s="72">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B9" s="71"/>
-      <c r="C9" s="72" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="87">
-        <v>35841976770</v>
-      </c>
-      <c r="E9" s="76">
-        <v>471831811</v>
-      </c>
-      <c r="F9" s="76">
-        <v>471929811</v>
-      </c>
-      <c r="G9" s="76">
-        <v>472145811</v>
-      </c>
-      <c r="H9" s="77">
-        <v>472157411</v>
-      </c>
-      <c r="I9" s="87">
-        <v>27984871336</v>
-      </c>
-      <c r="J9" s="76">
-        <v>436920153</v>
-      </c>
-      <c r="K9" s="76">
-        <v>436999453</v>
-      </c>
-      <c r="L9" s="76">
-        <v>437264453</v>
-      </c>
-      <c r="M9" s="77">
-        <v>437273953</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B10" s="71" t="s">
+      <c r="D10" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="E10" s="73"/>
+      <c r="F10" s="74">
+        <v>0.88</v>
+      </c>
+      <c r="G10" s="74">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H10" s="74">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I10" s="75">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="J10" s="73">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K10" s="74">
+        <v>0.89</v>
+      </c>
+      <c r="L10" s="74">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="M10" s="74">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="N10" s="75">
+        <v>0.89300000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="C11" s="67"/>
+      <c r="D11" s="68" t="s">
         <v>160</v>
       </c>
-      <c r="D10" s="78">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="E10" s="79">
+      <c r="E11" s="73"/>
+      <c r="F11" s="74">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="G11" s="74">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="H11" s="74">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="I11" s="75">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="J11" s="73">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K11" s="74">
+        <v>0.874</v>
+      </c>
+      <c r="L11" s="74">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="M11" s="74">
         <v>0.88</v>
       </c>
-      <c r="F10" s="79">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="G10" s="79">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="H10" s="80">
-        <v>0.88400000000000001</v>
-      </c>
-      <c r="I10" s="78">
-        <v>0.89</v>
-      </c>
-      <c r="J10" s="79">
-        <v>0.89</v>
-      </c>
-      <c r="K10" s="79">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="L10" s="79">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="M10" s="80">
+      <c r="N11" s="75">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="12" spans="3:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="C12" s="67"/>
+      <c r="D12" s="68" t="s">
+        <v>161</v>
+      </c>
+      <c r="E12" s="73"/>
+      <c r="F12" s="74">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G12" s="74">
+        <v>0.08</v>
+      </c>
+      <c r="H12" s="74">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I12" s="75">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J12" s="73">
         <v>0.89300000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B11" s="71"/>
-      <c r="C11" s="72" t="s">
-        <v>161</v>
-      </c>
-      <c r="D11" s="78">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="E11" s="79">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="F11" s="79">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="G11" s="79">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="H11" s="80">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="I11" s="78">
-        <v>0.874</v>
-      </c>
-      <c r="J11" s="79">
-        <v>0.874</v>
-      </c>
-      <c r="K11" s="79">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="L11" s="79">
-        <v>0.88</v>
-      </c>
-      <c r="M11" s="80">
-        <v>0.877</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="17" x14ac:dyDescent="0.2">
-      <c r="B12" s="71"/>
-      <c r="C12" s="72" t="s">
+      <c r="K12" s="74">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L12" s="74">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M12" s="74">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N12" s="75">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:17" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="76"/>
+      <c r="D13" s="77" t="s">
         <v>162</v>
       </c>
-      <c r="D12" s="78">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="E12" s="79">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="F12" s="79">
-        <v>0.08</v>
-      </c>
-      <c r="G12" s="79">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="H12" s="80">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="I12" s="78">
-        <v>1.6E-2</v>
-      </c>
-      <c r="J12" s="79">
-        <v>1.6E-2</v>
-      </c>
-      <c r="K12" s="79">
+      <c r="E13" s="78"/>
+      <c r="F13" s="79">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="L12" s="79">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="M12" s="80">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="81"/>
-      <c r="C13" s="82" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="83">
+      <c r="G13" s="79">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="H13" s="79">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="I13" s="80">
+        <v>0.01</v>
+      </c>
+      <c r="J13" s="78">
         <v>0.03</v>
       </c>
-      <c r="E13" s="84">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F13" s="84">
+      <c r="K13" s="79">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="G13" s="84">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="H13" s="85">
-        <v>0.01</v>
-      </c>
-      <c r="I13" s="83">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="J13" s="84">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="K13" s="84">
+      <c r="L13" s="79">
         <v>3.1E-2</v>
       </c>
-      <c r="L13" s="84">
+      <c r="M13" s="79">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="M13" s="85">
+      <c r="N13" s="80">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
+    <row r="14" spans="3:17" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="B4:C5"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="C4:D5"/>
+    <mergeCell ref="C3:N3"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C13"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DC479E-B3AC-EE45-96A7-4563B176590A}">
+  <dimension ref="B2:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q42" sqref="Q42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="94" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
+      <c r="F2" s="94"/>
+    </row>
+    <row r="3" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="91" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="91">
+        <v>54</v>
+      </c>
+      <c r="D3" s="91">
+        <v>55</v>
+      </c>
+      <c r="E3" s="91">
+        <v>56</v>
+      </c>
+      <c r="F3" s="92" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="93" t="s">
+        <v>171</v>
+      </c>
+      <c r="C4" s="93">
+        <v>1</v>
+      </c>
+      <c r="D4" s="93">
+        <v>2</v>
+      </c>
+      <c r="E4" s="93">
+        <v>15</v>
+      </c>
+      <c r="F4" s="93">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
now with raw M hifi
</commit_message>
<xml_diff>
--- a/tables_and_figures/Tables.xlsx
+++ b/tables_and_figures/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/tables_and_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FFFB4AB-9E72-954F-A6B4-FF8E693732BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02C820E-3F5E-8D4E-9460-4ECAEA6B2F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="6" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3561,8 +3561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0568C4-6AB0-0440-9F12-940870FA06A7}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G6"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4389,7 +4389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47DC479E-B3AC-EE45-96A7-4563B176590A}">
   <dimension ref="B2:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
up thru cyto rslts
</commit_message>
<xml_diff>
--- a/tables_and_figures/Tables.xlsx
+++ b/tables_and_figures/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/tables_and_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02C820E-3F5E-8D4E-9460-4ECAEA6B2F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D1C53F-407E-B64D-8218-D6598B54A652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="5" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -591,21 +591,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Table 4. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>Table of assembly steps with corresponding metrics. A0 = Metrics for unassembled, filtered PacBio HiFi reads; A1 = metrics after ipa assembly step; A2 = metrics afer scaffolding A1 assembly using linked-reads; A3 = metrics after scaffolding A2 assembly using hi-c data; A4 = metrics of final assembly resulting from anchoring chromosomes with a linkage map.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>A</t>
     </r>
     <r>
@@ -703,11 +688,29 @@
       <t xml:space="preserve"> Chromosome counts for delta smelt indicating 2n = 56.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Table 4. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>Table of assembly steps with corresponding metrics. A0 = Metrics for unassembled, filtered PacBio HiFi reads; A1 = metrics after ipa assembly step; A2 = metrics afer scaffolding A1 assembly using linked-reads; A3 = metrics after scaffolding A2 assembly using hi-c data; A4 = metrics of final assembly resulting from anchoring chromosomes with a linkage map. Continuity metrics created from genometools, BUSCO scores from comparison to August 05, 2020 Actinopterygii gene (n=3640) dataset.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="172" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1441,30 +1444,12 @@
     <xf numFmtId="3" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1505,6 +1490,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3561,8 +3564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0568C4-6AB0-0440-9F12-940870FA06A7}">
   <dimension ref="B2:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView zoomScale="109" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3995,8 +3998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF36CC-2E6B-0D43-87A8-02414AEC4EB5}">
   <dimension ref="C2:Q14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:N3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4004,9 +4007,10 @@
     <col min="1" max="1" width="10.83203125" style="14"/>
     <col min="2" max="2" width="2.6640625" style="14" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="14"/>
+    <col min="4" max="4" width="11.5" style="14" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="14" customWidth="1"/>
-    <col min="6" max="8" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="14" customWidth="1"/>
+    <col min="7" max="8" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
     <col min="11" max="13" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
@@ -4017,27 +4021,27 @@
   <sheetData>
     <row r="2" spans="3:17" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="3:17" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="D3" s="81"/>
-      <c r="E3" s="81"/>
-      <c r="F3" s="81"/>
-      <c r="G3" s="81"/>
-      <c r="H3" s="81"/>
-      <c r="I3" s="81"/>
-      <c r="J3" s="81"/>
-      <c r="K3" s="81"/>
-      <c r="L3" s="81"/>
-      <c r="M3" s="81"/>
-      <c r="N3" s="81"/>
-      <c r="Q3" s="84"/>
-    </row>
-    <row r="4" spans="3:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C3" s="75" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="Q3" s="78"/>
+    </row>
+    <row r="4" spans="3:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="D4" s="86"/>
+      <c r="D4" s="80"/>
       <c r="E4" s="58" t="s">
         <v>154</v>
       </c>
@@ -4045,7 +4049,7 @@
       <c r="G4" s="59"/>
       <c r="H4" s="59"/>
       <c r="I4" s="60"/>
-      <c r="J4" s="88" t="s">
+      <c r="J4" s="82" t="s">
         <v>155</v>
       </c>
       <c r="K4" s="59"/>
@@ -4053,38 +4057,38 @@
       <c r="M4" s="59"/>
       <c r="N4" s="60"/>
     </row>
-    <row r="5" spans="3:17" ht="19" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:17" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C5" s="61"/>
-      <c r="D5" s="85"/>
-      <c r="E5" s="87" t="s">
+      <c r="D5" s="79"/>
+      <c r="E5" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="F5" s="83" t="s">
         <v>166</v>
       </c>
-      <c r="F5" s="89" t="s">
+      <c r="G5" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="G5" s="89" t="s">
+      <c r="H5" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="H5" s="89" t="s">
+      <c r="I5" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="I5" s="90" t="s">
-        <v>170</v>
-      </c>
-      <c r="J5" s="87" t="s">
+      <c r="J5" s="81" t="s">
+        <v>165</v>
+      </c>
+      <c r="K5" s="83" t="s">
         <v>166</v>
       </c>
-      <c r="K5" s="89" t="s">
+      <c r="L5" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="L5" s="89" t="s">
+      <c r="M5" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="M5" s="89" t="s">
+      <c r="N5" s="84" t="s">
         <v>169</v>
-      </c>
-      <c r="N5" s="90" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="6" spans="3:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -4166,7 +4170,7 @@
       <c r="D8" s="68" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="77">
         <v>3095133</v>
       </c>
       <c r="F8" s="69">
@@ -4181,7 +4185,7 @@
       <c r="I8" s="68">
         <v>549</v>
       </c>
-      <c r="J8" s="83">
+      <c r="J8" s="77">
         <v>2741504</v>
       </c>
       <c r="K8" s="69">
@@ -4202,7 +4206,7 @@
       <c r="D9" s="68" t="s">
         <v>164</v>
       </c>
-      <c r="E9" s="82">
+      <c r="E9" s="76">
         <v>35145204844</v>
       </c>
       <c r="F9" s="71">
@@ -4217,7 +4221,7 @@
       <c r="I9" s="72">
         <v>472157411</v>
       </c>
-      <c r="J9" s="82">
+      <c r="J9" s="76">
         <v>27984871336</v>
       </c>
       <c r="K9" s="71">
@@ -4240,32 +4244,34 @@
       <c r="D10" s="68" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="74">
+      <c r="E10" s="89">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="F10" s="91">
         <v>0.88</v>
       </c>
-      <c r="G10" s="74">
+      <c r="G10" s="91">
         <v>0.88500000000000001</v>
       </c>
-      <c r="H10" s="74">
+      <c r="H10" s="91">
         <v>0.88200000000000001</v>
       </c>
-      <c r="I10" s="75">
+      <c r="I10" s="92">
         <v>0.88400000000000001</v>
       </c>
-      <c r="J10" s="73">
+      <c r="J10" s="89">
         <v>0.92600000000000005</v>
       </c>
-      <c r="K10" s="74">
+      <c r="K10" s="91">
         <v>0.89</v>
       </c>
-      <c r="L10" s="74">
+      <c r="L10" s="91">
         <v>0.85899999999999999</v>
       </c>
-      <c r="M10" s="74">
+      <c r="M10" s="91">
         <v>0.89500000000000002</v>
       </c>
-      <c r="N10" s="75">
+      <c r="N10" s="92">
         <v>0.89300000000000002</v>
       </c>
     </row>
@@ -4274,32 +4280,34 @@
       <c r="D11" s="68" t="s">
         <v>160</v>
       </c>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74">
+      <c r="E11" s="89">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F11" s="91">
         <v>0.79500000000000004</v>
       </c>
-      <c r="G11" s="74">
+      <c r="G11" s="91">
         <v>0.80500000000000005</v>
       </c>
-      <c r="H11" s="74">
+      <c r="H11" s="91">
         <v>0.80500000000000005</v>
       </c>
-      <c r="I11" s="75">
+      <c r="I11" s="92">
         <v>0.81200000000000006</v>
       </c>
-      <c r="J11" s="73">
+      <c r="J11" s="89">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="K11" s="74">
+      <c r="K11" s="91">
         <v>0.874</v>
       </c>
-      <c r="L11" s="74">
+      <c r="L11" s="91">
         <v>0.84399999999999997</v>
       </c>
-      <c r="M11" s="74">
+      <c r="M11" s="91">
         <v>0.88</v>
       </c>
-      <c r="N11" s="75">
+      <c r="N11" s="92">
         <v>0.877</v>
       </c>
     </row>
@@ -4308,66 +4316,70 @@
       <c r="D12" s="68" t="s">
         <v>161</v>
       </c>
-      <c r="E12" s="73"/>
-      <c r="F12" s="74">
+      <c r="E12" s="89">
+        <v>0.87</v>
+      </c>
+      <c r="F12" s="91">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="G12" s="74">
+      <c r="G12" s="91">
         <v>0.08</v>
       </c>
-      <c r="H12" s="74">
+      <c r="H12" s="91">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="I12" s="75">
+      <c r="I12" s="92">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="89">
         <v>0.89300000000000002</v>
       </c>
-      <c r="K12" s="74">
+      <c r="K12" s="91">
         <v>1.6E-2</v>
       </c>
-      <c r="L12" s="74">
+      <c r="L12" s="91">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M12" s="74">
+      <c r="M12" s="91">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="N12" s="75">
+      <c r="N12" s="92">
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="13" spans="3:17" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="76"/>
-      <c r="D13" s="77" t="s">
+      <c r="C13" s="73"/>
+      <c r="D13" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="E13" s="78"/>
-      <c r="F13" s="79">
+      <c r="E13" s="90">
+        <v>0.04</v>
+      </c>
+      <c r="F13" s="93">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G13" s="79">
+      <c r="G13" s="93">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H13" s="79">
+      <c r="H13" s="93">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I13" s="80">
+      <c r="I13" s="94">
         <v>0.01</v>
       </c>
-      <c r="J13" s="78">
+      <c r="J13" s="90">
         <v>0.03</v>
       </c>
-      <c r="K13" s="79">
+      <c r="K13" s="93">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L13" s="79">
+      <c r="L13" s="93">
         <v>3.1E-2</v>
       </c>
-      <c r="M13" s="79">
+      <c r="M13" s="93">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N13" s="80">
+      <c r="N13" s="94">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
@@ -4399,45 +4411,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="94" t="s">
-        <v>174</v>
-      </c>
-      <c r="C2" s="94"/>
-      <c r="D2" s="94"/>
-      <c r="E2" s="94"/>
-      <c r="F2" s="94"/>
+      <c r="B2" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
+      <c r="E2" s="88"/>
+      <c r="F2" s="88"/>
     </row>
     <row r="3" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="91" t="s">
+      <c r="B3" s="85" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="85">
+        <v>54</v>
+      </c>
+      <c r="D3" s="85">
+        <v>55</v>
+      </c>
+      <c r="E3" s="85">
+        <v>56</v>
+      </c>
+      <c r="F3" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="91">
-        <v>54</v>
-      </c>
-      <c r="D3" s="91">
-        <v>55</v>
-      </c>
-      <c r="E3" s="91">
-        <v>56</v>
-      </c>
-      <c r="F3" s="92" t="s">
-        <v>173</v>
-      </c>
     </row>
     <row r="4" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="93" t="s">
-        <v>171</v>
-      </c>
-      <c r="C4" s="93">
+      <c r="B4" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="87">
         <v>1</v>
       </c>
-      <c r="D4" s="93">
+      <c r="D4" s="87">
         <v>2</v>
       </c>
-      <c r="E4" s="93">
+      <c r="E4" s="87">
         <v>15</v>
       </c>
-      <c r="F4" s="93">
+      <c r="F4" s="87">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
up to DISCUSSION gasp
</commit_message>
<xml_diff>
--- a/tables_and_figures/Tables.xlsx
+++ b/tables_and_figures/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/tables_and_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D1C53F-407E-B64D-8218-D6598B54A652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C316B562-E982-6341-8642-FA73A93D8CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="5" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="176">
   <si>
     <t>Total sequence length</t>
   </si>
@@ -566,12 +566,6 @@
     <t>L50</t>
   </si>
   <si>
-    <t># contigs</t>
-  </si>
-  <si>
-    <t>BUSCO</t>
-  </si>
-  <si>
     <t>complete</t>
   </si>
   <si>
@@ -584,85 +578,7 @@
     <t>fragmented</t>
   </si>
   <si>
-    <t>Continuity Metrics</t>
-  </si>
-  <si>
     <t>total length</t>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-      </rPr>
-      <t>4</t>
-    </r>
   </si>
   <si>
     <t># Cells</t>
@@ -690,18 +606,100 @@
   </si>
   <si>
     <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light (Body)"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light (Body)"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light (Body)"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light (Body)"/>
+      </rPr>
+      <t>3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri Light (Body)"/>
+      </rPr>
+      <t>4</t>
+    </r>
+  </si>
+  <si>
+    <t>BUSCO
+Scores</t>
+  </si>
+  <si>
+    <t>Continuity
+Metrics</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">Table 4. </t>
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="major"/>
+        <rFont val="Calibri Light (Body)"/>
       </rPr>
-      <t>Table of assembly steps with corresponding metrics. A0 = Metrics for unassembled, filtered PacBio HiFi reads; A1 = metrics after ipa assembly step; A2 = metrics afer scaffolding A1 assembly using linked-reads; A3 = metrics after scaffolding A2 assembly using hi-c data; A4 = metrics of final assembly resulting from anchoring chromosomes with a linkage map. Continuity metrics created from genometools, BUSCO scores from comparison to August 05, 2020 Actinopterygii gene (n=3640) dataset.</t>
+      <t>Table of assembly steps with corresponding metrics. A0 = Metrics for unassembled, filtered PacBio HiFi reads; A1 = draft resulting from initial long-read assembly step; A2 = draft resulting from scaffolding A1 assembly using linked-reads; A3 = draft resulting from scaffolding A2 assembly using hi-c data; A4 = final assembly metrics resulting from anchoring chromosomes with a linkage map. Continuity metrics created from genometools, BUSCO scores from comparison to August 05, 2020 Actinopterygii gene (n=3640) dataset.</t>
     </r>
+  </si>
+  <si>
+    <t>N50 (bp)</t>
+  </si>
+  <si>
+    <t># contigs (bp)</t>
   </si>
 </sst>
 </file>
@@ -711,7 +709,7 @@
   <numFmts count="1">
     <numFmt numFmtId="172" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -833,17 +831,26 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
+      <name val="Calibri Light (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri Light (Body)"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri Light (Body)"/>
     </font>
     <font>
       <vertAlign val="subscript"/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri Light"/>
-      <family val="2"/>
+      <name val="Calibri Light (Body)"/>
     </font>
   </fonts>
   <fills count="5">
@@ -872,7 +879,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1188,10 +1195,32 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1235,15 +1264,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1282,7 +1302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1396,118 +1416,135 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="172" fontId="7" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="17" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="17" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="17" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="17" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="17" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="172" fontId="17" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3996,394 +4033,445 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF36CC-2E6B-0D43-87A8-02414AEC4EB5}">
-  <dimension ref="C2:Q14"/>
+  <dimension ref="B2:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="14"/>
-    <col min="2" max="2" width="2.6640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="11.5" style="14" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="11.1640625" style="14" customWidth="1"/>
-    <col min="7" max="8" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.1640625" style="14" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.1640625" style="14" customWidth="1"/>
-    <col min="15" max="15" width="2.83203125" style="14" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="14"/>
+    <col min="1" max="1" width="10.83203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="2.33203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="9" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="9.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.33203125" style="14" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="14"/>
+    <col min="17" max="17" width="12.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="14"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:17" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="3" spans="3:17" ht="52" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="75" t="s">
+    <row r="2" spans="2:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="62"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="63"/>
+      <c r="N2" s="63"/>
+      <c r="O2" s="64"/>
+    </row>
+    <row r="3" spans="2:17" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="65"/>
+      <c r="C3" s="66" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="67"/>
+      <c r="Q3" s="57"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B4" s="65"/>
+      <c r="C4" s="68" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="104"/>
+      <c r="E4" s="69" t="s">
+        <v>154</v>
+      </c>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="72" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
+      <c r="M4" s="70"/>
+      <c r="N4" s="71"/>
+      <c r="O4" s="67"/>
+    </row>
+    <row r="5" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="65"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="G5" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="H5" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="J5" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="K5" s="75" t="s">
+        <v>167</v>
+      </c>
+      <c r="L5" s="75" t="s">
+        <v>168</v>
+      </c>
+      <c r="M5" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="N5" s="76" t="s">
+        <v>170</v>
+      </c>
+      <c r="O5" s="67"/>
+    </row>
+    <row r="6" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="99"/>
+      <c r="C6" s="77" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" s="78" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
-      <c r="M3" s="75"/>
-      <c r="N3" s="75"/>
-      <c r="Q3" s="78"/>
-    </row>
-    <row r="4" spans="3:17" ht="23" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="58" t="s">
-        <v>154</v>
-      </c>
-      <c r="F4" s="59"/>
-      <c r="G4" s="59"/>
-      <c r="H4" s="59"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="82" t="s">
-        <v>155</v>
-      </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59"/>
-      <c r="M4" s="59"/>
-      <c r="N4" s="60"/>
-    </row>
-    <row r="5" spans="3:17" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="61"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="F5" s="83" t="s">
-        <v>166</v>
-      </c>
-      <c r="G5" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="83" t="s">
-        <v>168</v>
-      </c>
-      <c r="I5" s="84" t="s">
-        <v>169</v>
-      </c>
-      <c r="J5" s="81" t="s">
-        <v>165</v>
-      </c>
-      <c r="K5" s="83" t="s">
-        <v>166</v>
-      </c>
-      <c r="L5" s="83" t="s">
-        <v>167</v>
-      </c>
-      <c r="M5" s="83" t="s">
-        <v>168</v>
-      </c>
-      <c r="N5" s="84" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="6" spans="3:17" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="62" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="E6" s="64">
+      <c r="E6" s="79">
         <v>11604</v>
       </c>
-      <c r="F6" s="65">
+      <c r="F6" s="80">
         <v>353581</v>
       </c>
-      <c r="G6" s="65">
+      <c r="G6" s="80">
         <v>1188596</v>
       </c>
-      <c r="H6" s="65">
+      <c r="H6" s="80">
         <v>2749144</v>
       </c>
-      <c r="I6" s="66">
+      <c r="I6" s="81">
         <v>12200365</v>
       </c>
-      <c r="J6" s="64">
+      <c r="J6" s="79">
         <v>15048</v>
       </c>
-      <c r="K6" s="65">
+      <c r="K6" s="80">
         <v>418614</v>
       </c>
-      <c r="L6" s="65">
+      <c r="L6" s="80">
         <v>1392224</v>
       </c>
-      <c r="M6" s="65">
+      <c r="M6" s="80">
         <v>4383157</v>
       </c>
-      <c r="N6" s="66">
+      <c r="N6" s="81">
         <v>14850352</v>
       </c>
-    </row>
-    <row r="7" spans="3:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="C7" s="67"/>
-      <c r="D7" s="68" t="s">
+      <c r="O6" s="101"/>
+    </row>
+    <row r="7" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="99"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="83" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="70">
+      <c r="E7" s="84">
         <v>1276120</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="85">
         <v>324</v>
       </c>
-      <c r="G7" s="69">
+      <c r="G7" s="85">
         <v>106</v>
       </c>
-      <c r="H7" s="69">
+      <c r="H7" s="85">
         <v>38</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="83">
         <v>15</v>
       </c>
-      <c r="J7" s="70">
+      <c r="J7" s="84">
         <v>771808</v>
       </c>
-      <c r="K7" s="69">
+      <c r="K7" s="85">
         <v>264</v>
       </c>
-      <c r="L7" s="69">
+      <c r="L7" s="85">
         <v>80</v>
       </c>
-      <c r="M7" s="69">
+      <c r="M7" s="85">
         <v>26</v>
       </c>
-      <c r="N7" s="68">
+      <c r="N7" s="83">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="3:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="C8" s="67"/>
-      <c r="D8" s="68" t="s">
+      <c r="O7" s="101"/>
+    </row>
+    <row r="8" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="99"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="83" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="100">
+        <v>3095133</v>
+      </c>
+      <c r="F8" s="86">
+        <v>2086</v>
+      </c>
+      <c r="G8" s="86">
+        <v>1106</v>
+      </c>
+      <c r="H8" s="85">
+        <v>705</v>
+      </c>
+      <c r="I8" s="83">
+        <v>549</v>
+      </c>
+      <c r="J8" s="100">
+        <v>2741504</v>
+      </c>
+      <c r="K8" s="86">
+        <v>1805</v>
+      </c>
+      <c r="L8" s="86">
+        <v>1012</v>
+      </c>
+      <c r="M8" s="85">
+        <v>515</v>
+      </c>
+      <c r="N8" s="83">
+        <v>376</v>
+      </c>
+      <c r="O8" s="101"/>
+    </row>
+    <row r="9" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="99"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="83" t="s">
+        <v>161</v>
+      </c>
+      <c r="E9" s="103">
+        <v>35145204844</v>
+      </c>
+      <c r="F9" s="86">
+        <v>471831811</v>
+      </c>
+      <c r="G9" s="86">
+        <v>471929811</v>
+      </c>
+      <c r="H9" s="86">
+        <v>472145811</v>
+      </c>
+      <c r="I9" s="87">
+        <v>472157411</v>
+      </c>
+      <c r="J9" s="103">
+        <v>27984871336</v>
+      </c>
+      <c r="K9" s="86">
+        <v>436920153</v>
+      </c>
+      <c r="L9" s="86">
+        <v>436999453</v>
+      </c>
+      <c r="M9" s="86">
+        <v>437264453</v>
+      </c>
+      <c r="N9" s="87">
+        <v>437273953</v>
+      </c>
+      <c r="O9" s="101"/>
+    </row>
+    <row r="10" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="99"/>
+      <c r="C10" s="82" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="83" t="s">
         <v>157</v>
       </c>
-      <c r="E8" s="77">
-        <v>3095133</v>
-      </c>
-      <c r="F8" s="69">
-        <v>2086</v>
-      </c>
-      <c r="G8" s="69">
-        <v>1106</v>
-      </c>
-      <c r="H8" s="69">
-        <v>705</v>
-      </c>
-      <c r="I8" s="68">
-        <v>549</v>
-      </c>
-      <c r="J8" s="77">
-        <v>2741504</v>
-      </c>
-      <c r="K8" s="69">
-        <v>1805</v>
-      </c>
-      <c r="L8" s="69">
-        <v>1012</v>
-      </c>
-      <c r="M8" s="69">
-        <v>515</v>
-      </c>
-      <c r="N8" s="68">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="9" spans="3:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="C9" s="67"/>
-      <c r="D9" s="68" t="s">
-        <v>164</v>
-      </c>
-      <c r="E9" s="76">
-        <v>35145204844</v>
-      </c>
-      <c r="F9" s="71">
-        <v>471831811</v>
-      </c>
-      <c r="G9" s="71">
-        <v>471929811</v>
-      </c>
-      <c r="H9" s="71">
-        <v>472145811</v>
-      </c>
-      <c r="I9" s="72">
-        <v>472157411</v>
-      </c>
-      <c r="J9" s="76">
-        <v>27984871336</v>
-      </c>
-      <c r="K9" s="71">
-        <v>436920153</v>
-      </c>
-      <c r="L9" s="71">
-        <v>436999453</v>
-      </c>
-      <c r="M9" s="71">
-        <v>437264453</v>
-      </c>
-      <c r="N9" s="72">
-        <v>437273953</v>
-      </c>
-    </row>
-    <row r="10" spans="3:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="C10" s="67" t="s">
+      <c r="E10" s="88">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="F10" s="89">
+        <v>0.88</v>
+      </c>
+      <c r="G10" s="89">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="H10" s="89">
+        <v>0.88200000000000001</v>
+      </c>
+      <c r="I10" s="90">
+        <v>0.88400000000000001</v>
+      </c>
+      <c r="J10" s="88">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="K10" s="89">
+        <v>0.89</v>
+      </c>
+      <c r="L10" s="89">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="M10" s="89">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="N10" s="90">
+        <v>0.89300000000000002</v>
+      </c>
+      <c r="O10" s="101"/>
+    </row>
+    <row r="11" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="99"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="E11" s="88">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="F11" s="89">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="G11" s="89">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="H11" s="89">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="I11" s="90">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="J11" s="88">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="K11" s="89">
+        <v>0.874</v>
+      </c>
+      <c r="L11" s="89">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="M11" s="89">
+        <v>0.88</v>
+      </c>
+      <c r="N11" s="90">
+        <v>0.877</v>
+      </c>
+      <c r="O11" s="101"/>
+    </row>
+    <row r="12" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="99"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="89">
-        <v>0.90400000000000003</v>
-      </c>
-      <c r="F10" s="91">
-        <v>0.88</v>
-      </c>
-      <c r="G10" s="91">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="H10" s="91">
-        <v>0.88200000000000001</v>
-      </c>
-      <c r="I10" s="92">
-        <v>0.88400000000000001</v>
-      </c>
-      <c r="J10" s="89">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="K10" s="91">
-        <v>0.89</v>
-      </c>
-      <c r="L10" s="91">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="M10" s="91">
-        <v>0.89500000000000002</v>
-      </c>
-      <c r="N10" s="92">
+      <c r="E12" s="88">
+        <v>0.87</v>
+      </c>
+      <c r="F12" s="89">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G12" s="89">
+        <v>0.08</v>
+      </c>
+      <c r="H12" s="89">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I12" s="90">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="J12" s="88">
         <v>0.89300000000000002</v>
       </c>
-    </row>
-    <row r="11" spans="3:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="C11" s="67"/>
-      <c r="D11" s="68" t="s">
+      <c r="K12" s="89">
+        <v>1.6E-2</v>
+      </c>
+      <c r="L12" s="89">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M12" s="89">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N12" s="90">
+        <v>1.6E-2</v>
+      </c>
+      <c r="O12" s="101"/>
+    </row>
+    <row r="13" spans="2:17" s="102" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="99"/>
+      <c r="C13" s="91"/>
+      <c r="D13" s="92" t="s">
         <v>160</v>
       </c>
-      <c r="E11" s="89">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="F11" s="91">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="G11" s="91">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="H11" s="91">
-        <v>0.80500000000000005</v>
-      </c>
-      <c r="I11" s="92">
-        <v>0.81200000000000006</v>
-      </c>
-      <c r="J11" s="89">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="K11" s="91">
-        <v>0.874</v>
-      </c>
-      <c r="L11" s="91">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="M11" s="91">
-        <v>0.88</v>
-      </c>
-      <c r="N11" s="92">
-        <v>0.877</v>
-      </c>
-    </row>
-    <row r="12" spans="3:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="C12" s="67"/>
-      <c r="D12" s="68" t="s">
-        <v>161</v>
-      </c>
-      <c r="E12" s="89">
-        <v>0.87</v>
-      </c>
-      <c r="F12" s="91">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="G12" s="91">
-        <v>0.08</v>
-      </c>
-      <c r="H12" s="91">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="I12" s="92">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="J12" s="89">
-        <v>0.89300000000000002</v>
-      </c>
-      <c r="K12" s="91">
-        <v>1.6E-2</v>
-      </c>
-      <c r="L12" s="91">
+      <c r="E13" s="93">
+        <v>0.04</v>
+      </c>
+      <c r="F13" s="94">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="M12" s="91">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="N12" s="92">
-        <v>1.6E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:17" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="73"/>
-      <c r="D13" s="74" t="s">
-        <v>162</v>
-      </c>
-      <c r="E13" s="90">
-        <v>0.04</v>
-      </c>
-      <c r="F13" s="93">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="G13" s="93">
+      <c r="G13" s="94">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="H13" s="93">
+      <c r="H13" s="94">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="I13" s="94">
+      <c r="I13" s="95">
         <v>0.01</v>
       </c>
-      <c r="J13" s="90">
+      <c r="J13" s="93">
         <v>0.03</v>
       </c>
-      <c r="K13" s="93">
+      <c r="K13" s="94">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="L13" s="93">
+      <c r="L13" s="94">
         <v>3.1E-2</v>
       </c>
-      <c r="M13" s="93">
+      <c r="M13" s="94">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="N13" s="94">
+      <c r="N13" s="95">
         <v>8.0000000000000002E-3</v>
       </c>
-    </row>
-    <row r="14" spans="3:17" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="O13" s="101"/>
+    </row>
+    <row r="14" spans="2:17" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="97"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="97"/>
+      <c r="O14" s="98"/>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="E4:I4"/>
@@ -4411,45 +4499,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="88" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
-      <c r="E2" s="88"/>
-      <c r="F2" s="88"/>
+      <c r="B2" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
     </row>
     <row r="3" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="85" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="85">
+      <c r="B3" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="58">
         <v>54</v>
       </c>
-      <c r="D3" s="85">
+      <c r="D3" s="58">
         <v>55</v>
       </c>
-      <c r="E3" s="85">
+      <c r="E3" s="58">
         <v>56</v>
       </c>
-      <c r="F3" s="86" t="s">
-        <v>172</v>
+      <c r="F3" s="59" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="87" t="s">
-        <v>170</v>
-      </c>
-      <c r="C4" s="87">
+      <c r="B4" s="60" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="60">
         <v>1</v>
       </c>
-      <c r="D4" s="87">
+      <c r="D4" s="60">
         <v>2</v>
       </c>
-      <c r="E4" s="87">
+      <c r="E4" s="60">
         <v>15</v>
       </c>
-      <c r="F4" s="87">
+      <c r="F4" s="60">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
input ToC + citations
</commit_message>
<xml_diff>
--- a/tables_and_figures/Tables.xlsx
+++ b/tables_and_figures/Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/miocene/Desktop/git_repos/dissertation/tables_and_figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C316B562-E982-6341-8642-FA73A93D8CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8E4D98-2D75-AB48-94A4-8959CDA2A24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="5" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" activeTab="4" xr2:uid="{2DA336F4-BBFC-384B-89E7-86F75E70CA4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="184">
   <si>
     <t>Total sequence length</t>
   </si>
@@ -180,9 +180,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>run_ID</t>
-  </si>
-  <si>
     <t>m64069_201002_215024</t>
   </si>
   <si>
@@ -208,12 +205,6 @@
   </si>
   <si>
     <t>10X</t>
-  </si>
-  <si>
-    <t>R1</t>
-  </si>
-  <si>
-    <t>R2</t>
   </si>
   <si>
     <t>Q35</t>
@@ -700,6 +691,39 @@
   </si>
   <si>
     <t># contigs (bp)</t>
+  </si>
+  <si>
+    <t>Run ID</t>
+  </si>
+  <si>
+    <t>10X_R1_F</t>
+  </si>
+  <si>
+    <t>10X_R2_F</t>
+  </si>
+  <si>
+    <t>10X_R1_M</t>
+  </si>
+  <si>
+    <t>10X_R2_M</t>
+  </si>
+  <si>
+    <t>hic_R1_F</t>
+  </si>
+  <si>
+    <t>hic_R2_F</t>
+  </si>
+  <si>
+    <t>hic_R1_M</t>
+  </si>
+  <si>
+    <t>hic_R2_M</t>
+  </si>
+  <si>
+    <t>Phase Genomics Hi-C</t>
+  </si>
+  <si>
+    <t>VGP Hi-C</t>
   </si>
 </sst>
 </file>
@@ -2303,7 +2327,7 @@
     <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" s="36"/>
       <c r="C3" s="30" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D3" s="30"/>
       <c r="E3" s="30"/>
@@ -2331,13 +2355,13 @@
         <v>44</v>
       </c>
       <c r="E4" s="19" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H4" s="19" t="s">
         <v>28</v>
@@ -2364,13 +2388,13 @@
         <v>8</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="Q4" s="19" t="s">
         <v>10</v>
       </c>
       <c r="R4" s="20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="S4" s="37"/>
     </row>
@@ -2430,7 +2454,7 @@
         <v>22</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>24</v>
@@ -2577,7 +2601,7 @@
     <row r="9" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B9" s="36"/>
       <c r="C9" s="31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>43</v>
@@ -2694,7 +2718,7 @@
     <row r="3" spans="2:18" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="44"/>
       <c r="C3" s="45" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D3" s="45"/>
       <c r="E3" s="45"/>
@@ -2711,25 +2735,25 @@
         <v>44</v>
       </c>
       <c r="D4" s="47" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E4" s="47" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H4" s="47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="I4" s="47" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J4" s="47" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="K4" s="46"/>
     </row>
@@ -2739,16 +2763,16 @@
         <v>45</v>
       </c>
       <c r="D5" s="49" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E5" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F5" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G5" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H5" s="49"/>
       <c r="I5" s="49"/>
@@ -2759,21 +2783,21 @@
       <c r="B6" s="44"/>
       <c r="C6" s="48"/>
       <c r="D6" s="49" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F6" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G6" s="49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H6" s="49"/>
       <c r="I6" s="49"/>
       <c r="J6" s="49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K6" s="46"/>
     </row>
@@ -2781,16 +2805,16 @@
       <c r="B7" s="44"/>
       <c r="C7" s="48"/>
       <c r="D7" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>96</v>
-      </c>
       <c r="G7" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H7" s="49"/>
       <c r="I7" s="49"/>
@@ -2800,19 +2824,19 @@
     <row r="8" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="44"/>
       <c r="C8" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D8" s="49" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E8" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F8" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G8" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H8" s="49"/>
       <c r="I8" s="49"/>
@@ -2823,16 +2847,16 @@
       <c r="B9" s="44"/>
       <c r="C9" s="48"/>
       <c r="D9" s="49" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E9" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F9" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G9" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H9" s="49"/>
       <c r="I9" s="49"/>
@@ -2843,16 +2867,16 @@
       <c r="B10" s="44"/>
       <c r="C10" s="48"/>
       <c r="D10" s="49" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E10" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F10" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G10" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H10" s="49"/>
       <c r="I10" s="49"/>
@@ -2862,19 +2886,19 @@
     <row r="11" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="44"/>
       <c r="C11" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="49" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E11" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F11" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G11" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H11" s="49"/>
       <c r="I11" s="49"/>
@@ -2885,23 +2909,23 @@
       <c r="B12" s="44"/>
       <c r="C12" s="48"/>
       <c r="D12" s="49" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F12" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G12" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H12" s="49"/>
       <c r="I12" s="49"/>
       <c r="J12" s="49"/>
       <c r="K12" s="46"/>
       <c r="O12" s="53" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="P12"/>
       <c r="Q12"/>
@@ -2911,23 +2935,23 @@
       <c r="B13" s="44"/>
       <c r="C13" s="48"/>
       <c r="D13" s="49" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F13" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G13" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H13" s="49"/>
       <c r="I13" s="49"/>
       <c r="J13" s="49"/>
       <c r="K13" s="46"/>
       <c r="O13" s="53" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="P13"/>
       <c r="Q13"/>
@@ -2939,16 +2963,16 @@
         <v>45</v>
       </c>
       <c r="D14" s="49" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F14" s="49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G14" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H14" s="49"/>
       <c r="I14" s="49"/>
@@ -2963,16 +2987,16 @@
       <c r="B15" s="44"/>
       <c r="C15" s="48"/>
       <c r="D15" s="49" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F15" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G15" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H15" s="49"/>
       <c r="I15" s="49"/>
@@ -2987,48 +3011,48 @@
       <c r="B16" s="44"/>
       <c r="C16" s="48"/>
       <c r="D16" s="49" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="E16" s="49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F16" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G16" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H16" s="49"/>
       <c r="I16" s="49"/>
       <c r="J16" s="49"/>
       <c r="K16" s="46"/>
       <c r="O16" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="P16" s="55" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q16" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="R16" s="55" t="s">
         <v>121</v>
-      </c>
-      <c r="P16" s="55" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q16" s="55" t="s">
-        <v>123</v>
-      </c>
-      <c r="R16" s="55" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="17" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="44"/>
       <c r="C17" s="48"/>
       <c r="D17" s="49" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E17" s="49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F17" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G17" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H17" s="49"/>
       <c r="I17" s="49"/>
@@ -3043,23 +3067,23 @@
       <c r="B18" s="44"/>
       <c r="C18" s="48"/>
       <c r="D18" s="49" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E18" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F18" s="49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G18" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H18" s="49"/>
       <c r="I18" s="49"/>
       <c r="J18" s="49"/>
       <c r="K18" s="46"/>
       <c r="O18" s="54" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="P18" s="54">
         <v>1.87</v>
@@ -3068,30 +3092,30 @@
         <v>1.76</v>
       </c>
       <c r="R18" s="54" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="44"/>
       <c r="C19" s="48"/>
       <c r="D19" s="49" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F19" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G19" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H19" s="49"/>
       <c r="I19" s="49"/>
       <c r="J19" s="49"/>
       <c r="K19" s="46"/>
       <c r="O19" s="54" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="P19" s="54">
         <v>1.88</v>
@@ -3100,30 +3124,30 @@
         <v>1.53</v>
       </c>
       <c r="R19" s="54" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="44"/>
       <c r="C20" s="48"/>
       <c r="D20" s="49" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F20" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G20" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H20" s="49"/>
       <c r="I20" s="49"/>
       <c r="J20" s="49"/>
       <c r="K20" s="46"/>
       <c r="O20" s="54" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="P20" s="54">
         <v>1.73</v>
@@ -3132,32 +3156,32 @@
         <v>1.3</v>
       </c>
       <c r="R20" s="54" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="44"/>
       <c r="C21" s="48"/>
       <c r="D21" s="49" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F21" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G21" s="49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H21" s="49"/>
       <c r="I21" s="49"/>
       <c r="J21" s="49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K21" s="46"/>
       <c r="O21" s="54" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="P21" s="54">
         <v>1</v>
@@ -3166,32 +3190,32 @@
         <v>1.33</v>
       </c>
       <c r="R21" s="54" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="44"/>
       <c r="C22" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="49" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F22" s="49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G22" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H22" s="49"/>
       <c r="I22" s="49"/>
       <c r="J22" s="49"/>
       <c r="K22" s="46"/>
       <c r="O22" s="54" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="P22" s="54">
         <v>1.84</v>
@@ -3200,30 +3224,30 @@
         <v>2.2200000000000002</v>
       </c>
       <c r="R22" s="54" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="44"/>
       <c r="C23" s="48"/>
       <c r="D23" s="49" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="E23" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F23" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G23" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H23" s="49"/>
       <c r="I23" s="49"/>
       <c r="J23" s="49"/>
       <c r="K23" s="46"/>
       <c r="O23" s="54" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="P23" s="54">
         <v>1.26</v>
@@ -3232,30 +3256,30 @@
         <v>1.52</v>
       </c>
       <c r="R23" s="54" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="44"/>
       <c r="C24" s="48"/>
       <c r="D24" s="49" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E24" s="49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F24" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G24" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H24" s="49"/>
       <c r="I24" s="49"/>
       <c r="J24" s="49"/>
       <c r="K24" s="46"/>
       <c r="O24" s="54" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="P24" s="54">
         <v>1.84</v>
@@ -3264,30 +3288,30 @@
         <v>1.8</v>
       </c>
       <c r="R24" s="54" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="25" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="44"/>
       <c r="C25" s="48"/>
       <c r="D25" s="49" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F25" s="49" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G25" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H25" s="49"/>
       <c r="I25" s="49"/>
       <c r="J25" s="49"/>
       <c r="K25" s="46"/>
       <c r="O25" s="54" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="P25" s="54">
         <v>1.91</v>
@@ -3296,23 +3320,23 @@
         <v>2.02</v>
       </c>
       <c r="R25" s="54" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="44"/>
       <c r="C26" s="48"/>
       <c r="D26" s="49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E26" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F26" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G26" s="49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H26" s="49">
         <v>1.91</v>
@@ -3321,7 +3345,7 @@
         <v>2.02</v>
       </c>
       <c r="J26" s="49" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="K26" s="46"/>
       <c r="O26"/>
@@ -3333,16 +3357,16 @@
       <c r="B27" s="44"/>
       <c r="C27" s="48"/>
       <c r="D27" s="49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F27" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G27" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H27" s="49"/>
       <c r="I27" s="49"/>
@@ -3356,26 +3380,26 @@
     <row r="28" spans="2:18" ht="13" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B28" s="44"/>
       <c r="C28" s="48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D28" s="49" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="E28" s="49" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="F28" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G28" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H28" s="49"/>
       <c r="I28" s="49"/>
       <c r="J28" s="49"/>
       <c r="K28" s="46"/>
       <c r="O28" s="54" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="P28"/>
       <c r="Q28"/>
@@ -3385,25 +3409,25 @@
       <c r="B29" s="44"/>
       <c r="C29" s="48"/>
       <c r="D29" s="49" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E29" s="49" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F29" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G29" s="49" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="H29" s="49"/>
       <c r="I29" s="49"/>
       <c r="J29" s="49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K29" s="46"/>
       <c r="O29" s="54" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="P29"/>
       <c r="Q29"/>
@@ -3413,16 +3437,16 @@
       <c r="B30" s="44"/>
       <c r="C30" s="48"/>
       <c r="D30" s="49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E30" s="49" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F30" s="49" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="G30" s="49" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H30" s="49"/>
       <c r="I30" s="49"/>
@@ -3470,35 +3494,35 @@
   <sheetData>
     <row r="2" spans="2:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D3" s="23" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E4" s="26">
         <v>1</v>
@@ -3509,10 +3533,10 @@
     </row>
     <row r="5" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>45</v>
@@ -3526,13 +3550,13 @@
     </row>
     <row r="6" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E6" s="26">
         <v>2</v>
@@ -3543,10 +3567,10 @@
     </row>
     <row r="7" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="25" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D7" s="26" t="s">
         <v>45</v>
@@ -3560,10 +3584,10 @@
     </row>
     <row r="8" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D8" s="26" t="s">
         <v>45</v>
@@ -3572,24 +3596,24 @@
         <v>1</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="C9" s="26" t="s">
-        <v>108</v>
-      </c>
       <c r="D9" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" s="26">
         <v>1</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -3599,17 +3623,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0568C4-6AB0-0440-9F12-940870FA06A7}">
-  <dimension ref="B2:L24"/>
+  <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="14"/>
     <col min="2" max="2" width="3.83203125" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" style="14" customWidth="1"/>
+    <col min="3" max="3" width="18.5" style="14" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.1640625" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.83203125" style="14" customWidth="1"/>
     <col min="6" max="6" width="16.83203125" style="14" bestFit="1" customWidth="1"/>
@@ -3625,7 +3649,7 @@
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B2" s="29" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C2" s="29"/>
       <c r="D2" s="29"/>
@@ -3643,34 +3667,34 @@
         <v>44</v>
       </c>
       <c r="C3" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>46</v>
+        <v>173</v>
       </c>
       <c r="E3" s="28" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="F3" s="28" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G3" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="K3" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="28" t="s">
         <v>144</v>
-      </c>
-      <c r="H3" s="28" t="s">
-        <v>143</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>146</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="K3" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="L3" s="28" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.2">
@@ -3678,10 +3702,10 @@
         <v>45</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4" s="17">
         <v>7790139515</v>
@@ -3703,7 +3727,7 @@
       </c>
       <c r="K4" s="56"/>
       <c r="L4" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.2">
@@ -3711,10 +3735,10 @@
         <v>45</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D5" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E5" s="17">
         <v>6534076057</v>
@@ -3736,7 +3760,7 @@
       </c>
       <c r="K5" s="56"/>
       <c r="L5" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.2">
@@ -3744,10 +3768,10 @@
         <v>45</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D6" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" s="17">
         <v>14225369483</v>
@@ -3769,18 +3793,18 @@
       </c>
       <c r="K6" s="56"/>
       <c r="L6" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B7" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E7" s="17">
         <v>24466806025</v>
@@ -3798,18 +3822,18 @@
       <c r="J7" s="56"/>
       <c r="K7" s="56"/>
       <c r="L7" s="16" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E8" s="17">
         <v>11375170745</v>
@@ -3831,7 +3855,7 @@
       </c>
       <c r="K8" s="56"/>
       <c r="L8" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
@@ -3839,10 +3863,10 @@
         <v>45</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>56</v>
+        <v>174</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="17">
@@ -3866,10 +3890,10 @@
         <v>45</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>57</v>
+        <v>175</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="17">
@@ -3890,13 +3914,13 @@
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>56</v>
+        <v>176</v>
       </c>
       <c r="E11" s="17">
         <v>161450851775</v>
@@ -3919,13 +3943,13 @@
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B12" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>57</v>
+        <v>177</v>
       </c>
       <c r="E12" s="17">
         <v>161450851775</v>
@@ -3946,80 +3970,156 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E18" s="14">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="16"/>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="16"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="16"/>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="56"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="16"/>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="22" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E22" s="14">
         <v>1200000000</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F22" s="14">
         <v>490000000</v>
       </c>
-      <c r="G18" s="14" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E19" s="14">
-        <f>F9/E18</f>
+      <c r="G22" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E23" s="14">
+        <f>F9/E22</f>
         <v>79.021334848333339</v>
       </c>
-      <c r="F19" s="14">
-        <f>(F10/F18)/2</f>
+      <c r="F23" s="14">
+        <f>(F10/F22)/2</f>
         <v>96.760818181632658</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G23" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="H19" s="15">
+      <c r="H23" s="15">
         <f>SUM(F4:F6)</f>
         <v>27984871336</v>
       </c>
-      <c r="I19" s="14">
-        <f>(H19/490000000)/2</f>
+      <c r="I23" s="14">
+        <f>(H23/490000000)/2</f>
         <v>28.555991159183673</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K23" s="15">
         <f>SUM(H4:H6)</f>
         <v>2741504</v>
       </c>
-      <c r="L19" s="14">
+      <c r="L23" s="14">
         <v>2741504</v>
       </c>
     </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="E20" s="14">
-        <f>F11/E18</f>
+    <row r="24" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="E24" s="14">
+        <f>F11/E22</f>
         <v>54.838900778333333</v>
       </c>
-      <c r="F20" s="14">
-        <f>(F11/F18)/2</f>
+      <c r="F24" s="14">
+        <f>(F11/F22)/2</f>
         <v>67.149674422448982</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H20" s="15">
+      <c r="G24" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="15">
         <f>SUM(E7:E8)</f>
         <v>35841976770</v>
       </c>
-      <c r="I20" s="14">
-        <f>(H20/490000000)/2</f>
+      <c r="I24" s="14">
+        <f>(H24/490000000)/2</f>
         <v>36.573445683673469</v>
       </c>
-      <c r="K20" s="15">
+      <c r="K24" s="15">
         <f>SUM(H7:H8)</f>
         <v>3095133</v>
       </c>
-      <c r="L20" s="14">
+      <c r="L24" s="14">
         <v>3095133</v>
       </c>
     </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="H23" s="14">
+    <row r="27" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="H27" s="14">
         <v>27984871336</v>
       </c>
     </row>
-    <row r="24" spans="5:12" x14ac:dyDescent="0.2">
-      <c r="H24" s="14">
+    <row r="28" spans="5:12" x14ac:dyDescent="0.2">
+      <c r="H28" s="14">
         <v>35841976770</v>
       </c>
     </row>
@@ -4035,7 +4135,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CF36CC-2E6B-0D43-87A8-02414AEC4EB5}">
   <dimension ref="B2:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
@@ -4074,7 +4174,7 @@
     <row r="3" spans="2:17" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="65"/>
       <c r="C3" s="66" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D3" s="66"/>
       <c r="E3" s="66"/>
@@ -4093,18 +4193,18 @@
     <row r="4" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B4" s="65"/>
       <c r="C4" s="68" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="D4" s="104"/>
       <c r="E4" s="69" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="F4" s="70"/>
       <c r="G4" s="70"/>
       <c r="H4" s="70"/>
       <c r="I4" s="71"/>
       <c r="J4" s="72" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K4" s="70"/>
       <c r="L4" s="70"/>
@@ -4117,44 +4217,44 @@
       <c r="C5" s="73"/>
       <c r="D5" s="105"/>
       <c r="E5" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="H5" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="I5" s="76" t="s">
         <v>167</v>
       </c>
-      <c r="G5" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="H5" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="I5" s="76" t="s">
-        <v>170</v>
-      </c>
       <c r="J5" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="K5" s="75" t="s">
+        <v>164</v>
+      </c>
+      <c r="L5" s="75" t="s">
+        <v>165</v>
+      </c>
+      <c r="M5" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="K5" s="75" t="s">
+      <c r="N5" s="76" t="s">
         <v>167</v>
-      </c>
-      <c r="L5" s="75" t="s">
-        <v>168</v>
-      </c>
-      <c r="M5" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="N5" s="76" t="s">
-        <v>170</v>
       </c>
       <c r="O5" s="67"/>
     </row>
     <row r="6" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="99"/>
       <c r="C6" s="77" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D6" s="78" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="E6" s="79">
         <v>11604</v>
@@ -4192,7 +4292,7 @@
       <c r="B7" s="99"/>
       <c r="C7" s="82"/>
       <c r="D7" s="83" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E7" s="84">
         <v>1276120</v>
@@ -4230,7 +4330,7 @@
       <c r="B8" s="99"/>
       <c r="C8" s="82"/>
       <c r="D8" s="83" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E8" s="100">
         <v>3095133</v>
@@ -4268,7 +4368,7 @@
       <c r="B9" s="99"/>
       <c r="C9" s="82"/>
       <c r="D9" s="83" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="E9" s="103">
         <v>35145204844</v>
@@ -4305,10 +4405,10 @@
     <row r="10" spans="2:17" s="102" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B10" s="99"/>
       <c r="C10" s="82" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D10" s="83" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E10" s="88">
         <v>0.90400000000000003</v>
@@ -4346,7 +4446,7 @@
       <c r="B11" s="99"/>
       <c r="C11" s="82"/>
       <c r="D11" s="83" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E11" s="88">
         <v>3.4000000000000002E-2</v>
@@ -4384,7 +4484,7 @@
       <c r="B12" s="99"/>
       <c r="C12" s="82"/>
       <c r="D12" s="83" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E12" s="88">
         <v>0.87</v>
@@ -4422,7 +4522,7 @@
       <c r="B13" s="99"/>
       <c r="C13" s="91"/>
       <c r="D13" s="92" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="E13" s="93">
         <v>0.04</v>
@@ -4500,7 +4600,7 @@
   <sheetData>
     <row r="2" spans="2:6" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="61" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C2" s="61"/>
       <c r="D2" s="61"/>
@@ -4509,7 +4609,7 @@
     </row>
     <row r="3" spans="2:6" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="58" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C3" s="58">
         <v>54</v>
@@ -4521,12 +4621,12 @@
         <v>56</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="4" spans="2:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B4" s="60" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C4" s="60">
         <v>1</v>

</xml_diff>